<commit_message>
adding Adele to chart
</commit_message>
<xml_diff>
--- a/supervision.xlsx
+++ b/supervision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Documents/Long-Term-Projects-Files-For-Maintenance/htjb.github.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrybevins/Documents/Long-Term-Projects-For-Maintenance/htjb.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959AAEF9-CE54-D24A-9355-18B1B8ED984D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB703B1C-1973-3840-8B65-7B082B39D0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{C19BA659-2BE5-8443-A880-92F754B30969}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{C19BA659-2BE5-8443-A880-92F754B30969}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Supervision Style</t>
+  </si>
+  <si>
+    <t>Adele Chu</t>
   </si>
 </sst>
 </file>
@@ -579,10 +582,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -958,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0A7074-0E17-714A-A58A-70CC3CE49DF8}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1033,7 @@
       </c>
       <c r="I3" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -1044,7 +1048,7 @@
       </c>
       <c r="I4" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
@@ -1059,7 +1063,7 @@
       </c>
       <c r="I5" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
@@ -1080,7 +1084,7 @@
       </c>
       <c r="E6" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J6" t="s">
         <v>19</v>
@@ -1095,7 +1099,7 @@
       </c>
       <c r="I7" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
@@ -1110,7 +1114,7 @@
       </c>
       <c r="I8" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -1125,7 +1129,7 @@
       </c>
       <c r="G9" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -1140,7 +1144,7 @@
       </c>
       <c r="E10" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
@@ -1155,9 +1159,24 @@
       </c>
       <c r="E11" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45677.451944328706</v>
       </c>
       <c r="J11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45658</v>
+      </c>
+      <c r="G12" s="2">
+        <f ca="1">NOW()</f>
+        <v>45677.451944328706</v>
+      </c>
+      <c r="J12" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fiddling with supervision graph
</commit_message>
<xml_diff>
--- a/supervision.xlsx
+++ b/supervision.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Documents/Long-Term-Projects-Files-For-Maintenance/htjb.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959AAEF9-CE54-D24A-9355-18B1B8ED984D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A807DF-775E-B74E-BA72-784B850FE266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{C19BA659-2BE5-8443-A880-92F754B30969}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Supervision Style</t>
+  </si>
+  <si>
+    <t>Adele Chu</t>
   </si>
 </sst>
 </file>
@@ -958,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0A7074-0E17-714A-A58A-70CC3CE49DF8}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1017,7 @@
         <v>45200</v>
       </c>
       <c r="E2" s="1">
-        <v>45352</v>
+        <v>45444</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -1029,7 +1032,7 @@
       </c>
       <c r="I3" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -1044,7 +1047,7 @@
       </c>
       <c r="I4" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
@@ -1059,7 +1062,7 @@
       </c>
       <c r="I5" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
@@ -1079,8 +1082,8 @@
         <v>45566</v>
       </c>
       <c r="E6" s="2">
-        <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <f ca="1">MIN(NOW(), "01/06/2025  00:00:00")</f>
+        <v>45791.636239930558</v>
       </c>
       <c r="J6" t="s">
         <v>19</v>
@@ -1095,7 +1098,7 @@
       </c>
       <c r="I7" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
@@ -1110,7 +1113,7 @@
       </c>
       <c r="I8" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -1125,7 +1128,7 @@
       </c>
       <c r="G9" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <v>45791.636239930558</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -1139,8 +1142,8 @@
         <v>45566</v>
       </c>
       <c r="E10" s="2">
-        <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
+        <f ca="1">MIN(NOW(), "01/06/2025  00:00:00")</f>
+        <v>45791.636239930558</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
@@ -1154,10 +1157,25 @@
         <v>45566</v>
       </c>
       <c r="E11" s="2">
+        <f ca="1">MIN(NOW(), "01/06/2025  00:00:00")</f>
+        <v>45791.636239930558</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1">
+        <v>45658</v>
+      </c>
+      <c r="G12" s="2">
         <f ca="1">NOW()</f>
-        <v>45644.616621180554</v>
-      </c>
-      <c r="J11" t="s">
+        <v>45791.636239930558</v>
+      </c>
+      <c r="J12" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>